<commit_message>
I added some changes for night shift. There is still some little problems.
</commit_message>
<xml_diff>
--- a/ShiftSchedule.xlsx
+++ b/ShiftSchedule.xlsx
@@ -38,43 +38,43 @@
     <t>Sunday</t>
   </si>
   <si>
-    <t>asd</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>01.00-09.00</t>
   </si>
   <si>
     <t>Off</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>17.00-01.00</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>09.00-18.00</t>
   </si>
   <si>
-    <t>sd</t>
-  </si>
-  <si>
-    <t>17.00-01.00</t>
-  </si>
-  <si>
-    <t>01.00-09.00</t>
-  </si>
-  <si>
-    <t>ds</t>
-  </si>
-  <si>
-    <t>saa</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>sad</t>
-  </si>
-  <si>
-    <t>as</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>Week 2</t>
-  </si>
-  <si>
-    <t>IZINLI</t>
   </si>
   <si>
     <t>Week 3</t>
@@ -97,12 +97,22 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="31"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
@@ -112,16 +122,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="49"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="43"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
       </patternFill>
     </fill>
     <fill>
@@ -136,22 +136,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="31"/>
+        <fgColor indexed="43"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="14"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="43"/>
       </patternFill>
     </fill>
   </fills>
@@ -171,228 +161,228 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -442,13 +432,13 @@
         <v>9</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s" s="6">
         <v>10</v>
@@ -465,7 +455,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s" s="9">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s" s="10">
         <v>12</v>
@@ -477,36 +467,36 @@
         <v>12</v>
       </c>
       <c r="G3" t="s" s="13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s" s="14">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s" s="15">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s" s="16">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s" s="17">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s" s="18">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s" s="19">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s" s="20">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s" s="21">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -514,134 +504,134 @@
         <v>14</v>
       </c>
       <c r="B5" t="s" s="22">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s" s="23">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s" s="24">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s" s="25">
         <v>12</v>
       </c>
       <c r="F5" t="s" s="26">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s" s="27">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s" s="28">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s" s="29">
         <v>9</v>
       </c>
       <c r="C6" t="s" s="30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s" s="31">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s" s="32">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s" s="33">
         <v>10</v>
       </c>
       <c r="G6" t="s" s="34">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s" s="35">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s" s="36">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s" s="37">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s" s="38">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s" s="39">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s" s="40">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s" s="41">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s" s="42">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s" s="43">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s" s="44">
         <v>10</v>
       </c>
       <c r="D8" t="s" s="45">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s" s="46">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s" s="47">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s" s="48">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s" s="49">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s" s="50">
         <v>10</v>
       </c>
       <c r="C9" t="s" s="51">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s" s="52">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s" s="53">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s" s="54">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s" s="55">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s" s="56">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s" s="0">
         <v>1</v>
@@ -670,25 +660,25 @@
         <v>8</v>
       </c>
       <c r="B12" t="s" s="57">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s" s="58">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s" s="59">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s" s="60">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s" s="61">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s" s="62">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H12" t="s" s="63">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
@@ -696,51 +686,51 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="64">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s" s="65">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s" s="66">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s" s="67">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F13" t="s" s="68">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s" s="69">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s" s="70">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s" s="71">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s" s="72">
         <v>9</v>
       </c>
       <c r="D14" t="s" s="73">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s" s="74">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F14" t="s" s="75">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s" s="76">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s" s="77">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -748,22 +738,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s" s="78">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s" s="79">
         <v>12</v>
       </c>
       <c r="D15" t="s" s="80">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s" s="81">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s" s="82">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s" s="83">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H15" t="s" s="84">
         <v>12</v>
@@ -771,68 +761,68 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s" s="85">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s" s="86">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s" s="87">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s" s="88">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s" s="89">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G16" t="s" s="90">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s" s="91">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s" s="92">
         <v>10</v>
       </c>
       <c r="C17" t="s" s="93">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s" s="94">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s" s="95">
         <v>10</v>
       </c>
       <c r="F17" t="s" s="96">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s" s="97">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s" s="98">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s" s="99">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s" s="100">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s" s="101">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s" s="102">
         <v>9</v>
@@ -849,28 +839,28 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s" s="106">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s" s="107">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s" s="108">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s" s="109">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s" s="110">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s" s="111">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H19" t="s" s="112">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -907,19 +897,19 @@
         <v>12</v>
       </c>
       <c r="C22" t="s" s="114">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s" s="115">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s" s="116">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s" s="117">
         <v>12</v>
       </c>
       <c r="G22" t="s" s="118">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s" s="119">
         <v>12</v>
@@ -933,48 +923,48 @@
         <v>10</v>
       </c>
       <c r="C23" t="s" s="121">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s" s="122">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s" s="123">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F23" t="s" s="124">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G23" t="s" s="125">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H23" t="s" s="126">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s" s="127">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s" s="128">
         <v>10</v>
       </c>
       <c r="D24" t="s" s="129">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s" s="130">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s" s="131">
         <v>10</v>
       </c>
       <c r="G24" t="s" s="132">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H24" t="s" s="133">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25">
@@ -985,71 +975,71 @@
         <v>9</v>
       </c>
       <c r="C25" t="s" s="135">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s" s="136">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s" s="137">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s" s="138">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G25" t="s" s="139">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H25" t="s" s="140">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s" s="141">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s" s="142">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s" s="143">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E26" t="s" s="144">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F26" t="s" s="145">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G26" t="s" s="146">
         <v>10</v>
       </c>
       <c r="H26" t="s" s="147">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s" s="148">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s" s="149">
         <v>9</v>
       </c>
       <c r="D27" t="s" s="150">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s" s="151">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s" s="152">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G27" t="s" s="153">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H27" t="s" s="154">
         <v>10</v>
@@ -1057,54 +1047,54 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s" s="155">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s" s="156">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s" s="157">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s" s="158">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s" s="159">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s" s="160">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H28" t="s" s="161">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s" s="162">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s" s="163">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s" s="164">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s" s="165">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F29" t="s" s="166">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G29" t="s" s="167">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H29" t="s" s="168">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31">
@@ -1138,25 +1128,25 @@
         <v>8</v>
       </c>
       <c r="B32" t="s" s="169">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s" s="170">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s" s="171">
         <v>10</v>
       </c>
       <c r="E32" t="s" s="172">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F32" t="s" s="173">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s" s="174">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s" s="175">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33">
@@ -1164,51 +1154,51 @@
         <v>11</v>
       </c>
       <c r="B33" t="s" s="176">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s" s="177">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s" s="178">
         <v>10</v>
       </c>
       <c r="E33" t="s" s="179">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="s" s="180">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G33" t="s" s="181">
         <v>9</v>
       </c>
       <c r="H33" t="s" s="182">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s" s="183">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s" s="184">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s" s="185">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E34" t="s" s="186">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s" s="187">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G34" t="s" s="188">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H34" t="s" s="189">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
@@ -1216,129 +1206,129 @@
         <v>14</v>
       </c>
       <c r="B35" t="s" s="190">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s" s="191">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s" s="192">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s" s="193">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F35" t="s" s="194">
         <v>12</v>
       </c>
       <c r="G35" t="s" s="195">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H35" t="s" s="196">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s" s="197">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s" s="198">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s" s="199">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E36" t="s" s="200">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F36" t="s" s="201">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G36" t="s" s="202">
         <v>12</v>
       </c>
       <c r="H36" t="s" s="203">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s" s="204">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s" s="205">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D37" t="s" s="206">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E37" t="s" s="207">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F37" t="s" s="208">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G37" t="s" s="209">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H37" t="s" s="210">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s" s="211">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s" s="212">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s" s="213">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E38" t="s" s="214">
         <v>10</v>
       </c>
       <c r="F38" t="s" s="215">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G38" t="s" s="216">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H38" t="s" s="217">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s" s="218">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s" s="219">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D39" t="s" s="220">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E39" t="s" s="221">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F39" t="s" s="222">
         <v>9</v>
       </c>
       <c r="G39" t="s" s="223">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H39" t="s" s="224">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I added some changes shift schedule. There is still some little problems.
</commit_message>
<xml_diff>
--- a/ShiftSchedule.xlsx
+++ b/ShiftSchedule.xlsx
@@ -53,16 +53,16 @@
     <t>09.00-18.00</t>
   </si>
   <si>
-    <t>3</t>
+    <t>34</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
+    <t>17.00-01.00</t>
+  </si>
+  <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>17.00-01.00</t>
   </si>
   <si>
     <t>6</t>
@@ -160,229 +160,229 @@
   <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -429,7 +429,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s" s="3">
         <v>9</v>
@@ -438,13 +438,13 @@
         <v>9</v>
       </c>
       <c r="F2" t="s" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -452,25 +452,25 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s" s="9">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s" s="10">
         <v>12</v>
       </c>
       <c r="E3" t="s" s="11">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s" s="12">
         <v>12</v>
       </c>
       <c r="G3" t="s" s="13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -478,25 +478,25 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s" s="16">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s" s="17">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s" s="19">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s" s="20">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s" s="21">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -504,10 +504,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s" s="22">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s" s="23">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s" s="24">
         <v>12</v>
@@ -516,39 +516,39 @@
         <v>12</v>
       </c>
       <c r="F5" t="s" s="26">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s" s="27">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s" s="28">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s" s="29">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s" s="30">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s" s="31">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s" s="32">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s" s="33">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s" s="34">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s" s="35">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -556,7 +556,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s" s="36">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s" s="37">
         <v>10</v>
@@ -565,16 +565,16 @@
         <v>10</v>
       </c>
       <c r="E7" t="s" s="39">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s" s="40">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s" s="41">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s" s="42">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -582,25 +582,25 @@
         <v>18</v>
       </c>
       <c r="B8" t="s" s="43">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s" s="44">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s" s="45">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s" s="46">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s" s="47">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s" s="48">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s" s="49">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -608,25 +608,25 @@
         <v>19</v>
       </c>
       <c r="B9" t="s" s="50">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s" s="51">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s" s="52">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s" s="53">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s" s="54">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s" s="55">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s" s="56">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -669,16 +669,16 @@
         <v>12</v>
       </c>
       <c r="E12" t="s" s="60">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s" s="61">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s" s="62">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H12" t="s" s="63">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
@@ -686,25 +686,25 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="64">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s" s="65">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s" s="66">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s" s="67">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s" s="68">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s" s="69">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s" s="70">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -712,10 +712,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s" s="71">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s" s="72">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s" s="73">
         <v>10</v>
@@ -724,7 +724,7 @@
         <v>12</v>
       </c>
       <c r="F14" t="s" s="75">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s" s="76">
         <v>12</v>
@@ -741,48 +741,48 @@
         <v>10</v>
       </c>
       <c r="C15" t="s" s="79">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s" s="80">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s" s="81">
         <v>12</v>
       </c>
       <c r="F15" t="s" s="82">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s" s="83">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s" s="84">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s" s="85">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s" s="86">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s" s="87">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s" s="88">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s" s="89">
         <v>10</v>
       </c>
       <c r="G16" t="s" s="90">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H16" t="s" s="91">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
@@ -790,25 +790,25 @@
         <v>17</v>
       </c>
       <c r="B17" t="s" s="92">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s" s="93">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s" s="94">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s" s="95">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s" s="96">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s" s="97">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H17" t="s" s="98">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
@@ -816,25 +816,25 @@
         <v>18</v>
       </c>
       <c r="B18" t="s" s="99">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s" s="100">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s" s="101">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s" s="102">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s" s="103">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G18" t="s" s="104">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H18" t="s" s="105">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -842,25 +842,25 @@
         <v>19</v>
       </c>
       <c r="B19" t="s" s="106">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s" s="107">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s" s="108">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s" s="109">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s" s="110">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s" s="111">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s" s="112">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -920,13 +920,13 @@
         <v>11</v>
       </c>
       <c r="B23" t="s" s="120">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s" s="121">
         <v>12</v>
       </c>
       <c r="D23" t="s" s="122">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s" s="123">
         <v>12</v>
@@ -946,25 +946,25 @@
         <v>13</v>
       </c>
       <c r="B24" t="s" s="127">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s" s="128">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s" s="129">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E24" t="s" s="130">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s" s="131">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G24" t="s" s="132">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H24" t="s" s="133">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
@@ -972,51 +972,51 @@
         <v>14</v>
       </c>
       <c r="B25" t="s" s="134">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s" s="135">
         <v>12</v>
       </c>
       <c r="D25" t="s" s="136">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s" s="137">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" t="s" s="138">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s" s="139">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H25" t="s" s="140">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s" s="141">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s" s="142">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s" s="143">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s" s="144">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F26" t="s" s="145">
         <v>12</v>
       </c>
       <c r="G26" t="s" s="146">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H26" t="s" s="147">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27">
@@ -1030,19 +1030,19 @@
         <v>9</v>
       </c>
       <c r="D27" t="s" s="150">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s" s="151">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s" s="152">
         <v>9</v>
       </c>
       <c r="G27" t="s" s="153">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H27" t="s" s="154">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -1050,25 +1050,25 @@
         <v>18</v>
       </c>
       <c r="B28" t="s" s="155">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s" s="156">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s" s="157">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s" s="158">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F28" t="s" s="159">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G28" t="s" s="160">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H28" t="s" s="161">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
@@ -1076,19 +1076,19 @@
         <v>19</v>
       </c>
       <c r="B29" t="s" s="162">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s" s="163">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s" s="164">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E29" t="s" s="165">
         <v>10</v>
       </c>
       <c r="F29" t="s" s="166">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G29" t="s" s="167">
         <v>12</v>
@@ -1128,19 +1128,19 @@
         <v>8</v>
       </c>
       <c r="B32" t="s" s="169">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s" s="170">
         <v>12</v>
       </c>
       <c r="D32" t="s" s="171">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E32" t="s" s="172">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F32" t="s" s="173">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G32" t="s" s="174">
         <v>12</v>
@@ -1154,25 +1154,25 @@
         <v>11</v>
       </c>
       <c r="B33" t="s" s="176">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s" s="177">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s" s="178">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E33" t="s" s="179">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F33" t="s" s="180">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G33" t="s" s="181">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H33" t="s" s="182">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34">
@@ -1180,16 +1180,16 @@
         <v>13</v>
       </c>
       <c r="B34" t="s" s="183">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s" s="184">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s" s="185">
         <v>12</v>
       </c>
       <c r="E34" t="s" s="186">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F34" t="s" s="187">
         <v>12</v>
@@ -1212,13 +1212,13 @@
         <v>9</v>
       </c>
       <c r="D35" t="s" s="192">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E35" t="s" s="193">
         <v>9</v>
       </c>
       <c r="F35" t="s" s="194">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G35" t="s" s="195">
         <v>9</v>
@@ -1229,28 +1229,28 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s" s="197">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s" s="198">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D36" t="s" s="199">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s" s="200">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" t="s" s="201">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G36" t="s" s="202">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H36" t="s" s="203">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37">
@@ -1258,25 +1258,25 @@
         <v>17</v>
       </c>
       <c r="B37" t="s" s="204">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s" s="205">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D37" t="s" s="206">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s" s="207">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s" s="208">
         <v>10</v>
       </c>
       <c r="G37" t="s" s="209">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H37" t="s" s="210">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38">
@@ -1284,25 +1284,25 @@
         <v>18</v>
       </c>
       <c r="B38" t="s" s="211">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s" s="212">
         <v>10</v>
       </c>
       <c r="D38" t="s" s="213">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E38" t="s" s="214">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F38" t="s" s="215">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G38" t="s" s="216">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H38" t="s" s="217">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
@@ -1310,25 +1310,25 @@
         <v>19</v>
       </c>
       <c r="B39" t="s" s="218">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s" s="219">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D39" t="s" s="220">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E39" t="s" s="221">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s" s="222">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G39" t="s" s="223">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H39" t="s" s="224">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>